<commit_message>
webscrapping da trilha de data scientist
</commit_message>
<xml_diff>
--- a/data/arquivo.xlsx
+++ b/data/arquivo.xlsx
@@ -11,6 +11,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cursos" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trilhas_tem_Cursos" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Membros_feadev" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="membro_feadev_faz_trilhas" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="membro_feadev_faz_cursos" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -464,12 +466,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Data Engineering</t>
+          <t>Associate Data Scientist in Python</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/associate-data-engineer-in-sql</t>
+          <t>https://app.datacamp.com/learn/career-tracks/associate-data-scientist-in-python</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -482,12 +484,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Associate Data Engineer in SQL</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/associate-data-scientist-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/associate-data-engineer-in-sql</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -500,7 +502,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Trilha FeaDev</t>
+          <t>Capacitação 2025 - Básico</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -519,7 +521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,6 +540,11 @@
           <t>nome_curso</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>duracao</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,6 +555,9 @@
           <t>Introduction to Python</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -557,6 +567,9 @@
         <is>
           <t>Intermediate Python</t>
         </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -567,6 +580,9 @@
         <is>
           <t>SQL</t>
         </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +633,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -632,7 +648,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -647,7 +663,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
@@ -837,4 +853,180 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id_membro</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id_trilha</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>data_inicio</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>data_fim</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>finalizado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15/06/2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20/06/2025</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id_membro</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id_curso</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>data_inicio</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>data_fim</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>finalizado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15/06/2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>15/06/2025</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>21/06/2025</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20/06/2025</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>21/06/2025</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agora faz associação entre trilhas e cursos
</commit_message>
<xml_diff>
--- a/data/arquivo.xlsx
+++ b/data/arquivo.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,12 +466,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Associate Data Scientist in Python</t>
+          <t>Applied Finance in Python</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/associate-data-scientist-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/applied-finance-in-python</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -484,12 +484,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Associate Data Engineer in SQL</t>
+          <t>Associate Data Scientist  in Python</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/associate-data-engineer-in-sql</t>
+          <t>https://app.datacamp.com/learn/career-tracks/associate-data-scientist-in-python</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -502,12 +502,106 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Capacitação 2025 - Básico</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>Excel Fundamentals</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/excel-fundamentals</t>
+        </is>
+      </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Finance Fundamentals in Python</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/finance-fundamentals-in-python</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Git Fundamentals</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/git-fundamentals</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Machine Learning Scientist in Python</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/machine-learning-scientist-in-python</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SQL Fundamentals</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/sql-fundamentals</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Time Series in Python</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/time-series-in-python</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,6 +639,11 @@
           <t>duracao</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -552,11 +651,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Introduction to Python</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
+          <t>Introduction to Portfolio Risk Management in Python</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-portfolio-risk-management-in-python</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -565,11 +671,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Intermediate Python</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
+          <t>Quantitative Risk Management in Python</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/quantitative-risk-management-in-python</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -578,11 +691,1334 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SQL</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+          <t>Credit Risk Modeling in Python</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/credit-risk-modeling-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GARCH Models in Python</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/garch-models-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Introduction to Python</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Intermediate Python</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/intermediate-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Data Manipulation with pandas</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/data-manipulation-with-pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Joining Data with pandas</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/joining-data-with-pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Introduction to Statistics in Python</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-statistics-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Introduction to Data Visualization with Matplotlib</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-data-visualization-with-matplotlib</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Introduction to Data Visualization with Seaborn</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-data-visualization-with-seaborn</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Introduction to Functions in Python</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-functions-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Python Toolbox</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/python-toolbox</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Exploratory Data Analysis in Python</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/exploratory-data-analysis-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Working with Categorical Data in Python</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/working-with-categorical-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Data Communication Concepts</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/data-communication-concepts</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Introduction to Importing Data in Python</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-importing-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Cleaning Data in Python</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/cleaning-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Working with Dates and Times in Python</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/working-with-dates-and-times-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Writing Functions in Python</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/writing-functions-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Introduction to Regression with statsmodels in Python</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-regression-with-statsmodels-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Sampling in Python</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/sampling-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Hypothesis Testing in Python</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/hypothesis-testing-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Experimental Design in Python</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/experimental-design-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Supervised Learning with scikit-learn</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/supervised-learning-with-scikit-learn</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Unsupervised Learning in Python</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/unsupervised-learning-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Machine Learning with Tree-Based Models in Python</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>5 hr</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-with-tree-based-models-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Introduction to Excel</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Data Preparation in Excel</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/data-preparation-in-excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Data Visualization in Excel</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/data-visualization-in-excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Data Analysis in Excel</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/data-analysis-in-excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Case Study: Analyzing Customer Churn in Excel</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/case-study:-analyzing-customer-churn-in-excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Introduction to Python for Finance</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-python-for-finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Intermediate Python for Finance</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/intermediate-python-for-finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Introduction to Financial Concepts in Python</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-financial-concepts-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Manipulating Time Series Data in Python</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/manipulating-time-series-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Importing and Managing Financial Data in Python</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>5 hr</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/importing-and-managing-financial-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Introduction to Portfolio Analysis in Python</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-portfolio-analysis-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Introduction to Git</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2 hr</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-git</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Intermediate Git</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2 hr</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/intermediate-git</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Advanced Git</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/advanced-git</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Linear Classifiers in Python</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/linear-classifiers-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Extreme Gradient Boosting with XGBoost</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/extreme-gradient-boosting-with-xgboost</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Cluster Analysis in Python</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/cluster-analysis-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction in Python</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/dimensionality-reduction-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Preprocessing for Machine Learning in Python</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/preprocessing-for-machine-learning-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Machine Learning for Time Series Data in Python</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-for-time-series-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Feature Engineering for Machine Learning in Python</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-machine-learning-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Model Validation in Python</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/model-validation-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Hyperparameter Tuning in Python</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/hyperparameter-tuning-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Introduction to Natural Language Processing in Python</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-natural-language-processing-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Natural Language Processing with spaCy</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/natural-language-processing-with-spacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Feature Engineering for NLP in Python</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-nlp-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Introduction to Deep Learning with PyTorch</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-deep-learning-with-pytorch</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Intermediate Deep Learning with PyTorch</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/intermediate-deep-learning-with-pytorch</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Image Processing in Python</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/image-processing-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Introduction to PySpark</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-pyspark</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Machine Learning with PySpark</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-with-pyspark</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Winning a Kaggle Competition in Python</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/winning-a-kaggle-competition-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Introduction to SQL</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2 hr</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Intermediate SQL</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/intermediate-sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Joining Data in SQL</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/joining-data-in-sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Data Manipulation in SQL</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/data-manipulation-in-sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>PostgreSQL Summary Stats and Window Functions</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/postgresql-summary-stats-and-window-functions</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Functions for Manipulating Data in PostgreSQL</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/functions-for-manipulating-data-in-postgresql</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Database Design</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/database-design</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Time Series Analysis in Python</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/time-series-analysis-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Visualizing Time Series Data in Python</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/visualizing-time-series-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ARIMA Models in Python</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/arima-models-in-python</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -596,7 +2032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,15 +2053,10 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ordem_curso</t>
+          <t>data_final_para_assistir</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>data_final_para_assistir</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>obrigatoriedade_curso</t>
         </is>
@@ -638,11 +2069,8 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -653,83 +2081,872 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>20/06/2023</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>20/06/2023</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="n">
+        <v>23</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
         <v>2</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B29" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
         <v>2</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>23/06/2023</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+      <c r="B30" t="n">
+        <v>28</v>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2</v>
+      </c>
+      <c r="B31" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2</v>
+      </c>
+      <c r="B33" t="n">
+        <v>31</v>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" t="n">
+        <v>32</v>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" t="n">
+        <v>33</v>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" t="n">
+        <v>34</v>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3</v>
+      </c>
+      <c r="B37" t="n">
+        <v>35</v>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" t="n">
+        <v>36</v>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>3</v>
+      </c>
+      <c r="B39" t="n">
+        <v>37</v>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" t="n">
+        <v>38</v>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" t="n">
+        <v>39</v>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" t="n">
+        <v>40</v>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>5</v>
+      </c>
+      <c r="B43" t="n">
+        <v>24</v>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>5</v>
+      </c>
+      <c r="B44" t="n">
+        <v>25</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>5</v>
+      </c>
+      <c r="B45" t="n">
+        <v>41</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>5</v>
+      </c>
+      <c r="B46" t="n">
+        <v>26</v>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>5</v>
+      </c>
+      <c r="B47" t="n">
+        <v>42</v>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>5</v>
+      </c>
+      <c r="B48" t="n">
+        <v>43</v>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>5</v>
+      </c>
+      <c r="B49" t="n">
+        <v>44</v>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>5</v>
+      </c>
+      <c r="B50" t="n">
+        <v>45</v>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>5</v>
+      </c>
+      <c r="B51" t="n">
+        <v>46</v>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>5</v>
+      </c>
+      <c r="B52" t="n">
+        <v>47</v>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>5</v>
+      </c>
+      <c r="B53" t="n">
+        <v>48</v>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>5</v>
+      </c>
+      <c r="B54" t="n">
+        <v>49</v>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>5</v>
+      </c>
+      <c r="B55" t="n">
+        <v>50</v>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>5</v>
+      </c>
+      <c r="B56" t="n">
+        <v>51</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>5</v>
+      </c>
+      <c r="B57" t="n">
+        <v>52</v>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>5</v>
+      </c>
+      <c r="B58" t="n">
+        <v>53</v>
+      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>5</v>
+      </c>
+      <c r="B59" t="n">
+        <v>54</v>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>5</v>
+      </c>
+      <c r="B60" t="n">
+        <v>55</v>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>5</v>
+      </c>
+      <c r="B61" t="n">
+        <v>56</v>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>5</v>
+      </c>
+      <c r="B62" t="n">
+        <v>57</v>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>5</v>
+      </c>
+      <c r="B63" t="n">
+        <v>58</v>
+      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>6</v>
+      </c>
+      <c r="B64" t="n">
+        <v>59</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>6</v>
+      </c>
+      <c r="B65" t="n">
+        <v>60</v>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>6</v>
+      </c>
+      <c r="B66" t="n">
+        <v>61</v>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>6</v>
+      </c>
+      <c r="B67" t="n">
+        <v>62</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>6</v>
+      </c>
+      <c r="B68" t="n">
+        <v>63</v>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>6</v>
+      </c>
+      <c r="B69" t="n">
+        <v>64</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>6</v>
+      </c>
+      <c r="B70" t="n">
+        <v>65</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>7</v>
+      </c>
+      <c r="B71" t="n">
+        <v>35</v>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>7</v>
+      </c>
+      <c r="B72" t="n">
+        <v>66</v>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>7</v>
+      </c>
+      <c r="B73" t="n">
+        <v>67</v>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>7</v>
+      </c>
+      <c r="B74" t="n">
+        <v>68</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>7</v>
+      </c>
+      <c r="B75" t="n">
+        <v>46</v>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusão da Capacitação básica 2025
</commit_message>
<xml_diff>
--- a/data/arquivo.xlsx
+++ b/data/arquivo.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,16 +502,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Excel Fundamentals</t>
+          <t>Capacitação Básica 2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/excel-fundamentals</t>
+          <t>https://app.datacamp.com/learn/career-tracks/capacitação-básica-2025</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -520,12 +520,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Finance Fundamentals in Python</t>
+          <t>Excel Fundamentals</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/finance-fundamentals-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/excel-fundamentals</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -538,12 +538,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Git Fundamentals</t>
+          <t>Finance Fundamentals in Python</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/git-fundamentals</t>
+          <t>https://app.datacamp.com/learn/career-tracks/finance-fundamentals-in-python</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -556,12 +556,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Machine Learning Scientist in Python</t>
+          <t>Git Fundamentals</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/machine-learning-scientist-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/git-fundamentals</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -574,12 +574,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SQL Fundamentals</t>
+          <t>Machine Learning Scientist in Python</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/sql-fundamentals</t>
+          <t>https://app.datacamp.com/learn/career-tracks/machine-learning-scientist-in-python</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -592,15 +592,33 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>SQL Fundamentals</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/sql-fundamentals</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Time Series in Python</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>https://app.datacamp.com/learn/career-tracks/time-series-in-python</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -615,7 +633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1191,17 +1209,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Introduction to Excel</t>
+          <t>Introduction to Git</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>2 hr</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-excel</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-git</t>
         </is>
       </c>
     </row>
@@ -1211,17 +1229,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Data Preparation in Excel</t>
+          <t>Introduction to Data Visualization with Plotly in Python</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>3 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-preparation-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-data-visualization-with-plotly-in-python</t>
         </is>
       </c>
     </row>
@@ -1231,17 +1249,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Data Visualization in Excel</t>
+          <t>Intermediate Git</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>3 hr</t>
+          <t>2 hr</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-visualization-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-git</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1269,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Data Analysis in Excel</t>
+          <t>Introduction to Object-Oriented Programming in Python</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1261,7 +1279,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-analysis-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-object-oriented-programming-in-python</t>
         </is>
       </c>
     </row>
@@ -1271,13 +1289,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Case Study: Analyzing Customer Churn in Excel</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
+          <t>Intermediate Object-Oriented Programming in Python</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/case-study:-analyzing-customer-churn-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-object-oriented-programming-in-python</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1309,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Introduction to Python for Finance</t>
+          <t>Web Scraping in Python</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1297,7 +1319,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-python-for-finance</t>
+          <t>https://app.datacamp.com/learn/courses/web-scraping-in-python</t>
         </is>
       </c>
     </row>
@@ -1307,17 +1329,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Intermediate Python for Finance</t>
+          <t>Introduction to SQL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>2 hr</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-python-for-finance</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-sql</t>
         </is>
       </c>
     </row>
@@ -1327,7 +1349,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Introduction to Financial Concepts in Python</t>
+          <t>Intermediate SQL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1337,7 +1359,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-financial-concepts-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-sql</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1369,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Manipulating Time Series Data in Python</t>
+          <t>Joining Data in SQL</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1357,7 +1379,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/manipulating-time-series-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/joining-data-in-sql</t>
         </is>
       </c>
     </row>
@@ -1367,17 +1389,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Importing and Managing Financial Data in Python</t>
+          <t>Introduction to Excel</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>5 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/importing-and-managing-financial-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-excel</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1409,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Introduction to Portfolio Analysis in Python</t>
+          <t>Data Preparation in Excel</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-portfolio-analysis-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/data-preparation-in-excel</t>
         </is>
       </c>
     </row>
@@ -1407,17 +1429,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Introduction to Git</t>
+          <t>Data Visualization in Excel</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-git</t>
+          <t>https://app.datacamp.com/learn/courses/data-visualization-in-excel</t>
         </is>
       </c>
     </row>
@@ -1427,17 +1449,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Intermediate Git</t>
+          <t>Data Analysis in Excel</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-git</t>
+          <t>https://app.datacamp.com/learn/courses/data-analysis-in-excel</t>
         </is>
       </c>
     </row>
@@ -1447,17 +1469,13 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Advanced Git</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>3 hr</t>
-        </is>
-      </c>
+          <t>Case Study: Analyzing Customer Churn in Excel</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/advanced-git</t>
+          <t>https://app.datacamp.com/learn/courses/case-study:-analyzing-customer-churn-in-excel</t>
         </is>
       </c>
     </row>
@@ -1467,7 +1485,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Linear Classifiers in Python</t>
+          <t>Introduction to Python for Finance</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1477,7 +1495,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/linear-classifiers-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-python-for-finance</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1505,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Extreme Gradient Boosting with XGBoost</t>
+          <t>Intermediate Python for Finance</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1497,7 +1515,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/extreme-gradient-boosting-with-xgboost</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-python-for-finance</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1525,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cluster Analysis in Python</t>
+          <t>Introduction to Financial Concepts in Python</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1517,7 +1535,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/cluster-analysis-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-financial-concepts-in-python</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1545,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Dimensionality Reduction in Python</t>
+          <t>Manipulating Time Series Data in Python</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1537,7 +1555,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/dimensionality-reduction-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/manipulating-time-series-data-in-python</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1565,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Preprocessing for Machine Learning in Python</t>
+          <t>Importing and Managing Financial Data in Python</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>5 hr</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/preprocessing-for-machine-learning-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/importing-and-managing-financial-data-in-python</t>
         </is>
       </c>
     </row>
@@ -1567,7 +1585,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Machine Learning for Time Series Data in Python</t>
+          <t>Introduction to Portfolio Analysis in Python</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1577,7 +1595,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/machine-learning-for-time-series-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-portfolio-analysis-in-python</t>
         </is>
       </c>
     </row>
@@ -1587,17 +1605,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Feature Engineering for Machine Learning in Python</t>
+          <t>Advanced Git</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-machine-learning-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/advanced-git</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1625,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Model Validation in Python</t>
+          <t>Linear Classifiers in Python</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1617,7 +1635,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/model-validation-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/linear-classifiers-in-python</t>
         </is>
       </c>
     </row>
@@ -1627,7 +1645,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Hyperparameter Tuning in Python</t>
+          <t>Extreme Gradient Boosting with XGBoost</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1637,7 +1655,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/hyperparameter-tuning-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/extreme-gradient-boosting-with-xgboost</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1665,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Introduction to Natural Language Processing in Python</t>
+          <t>Cluster Analysis in Python</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1657,7 +1675,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-natural-language-processing-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/cluster-analysis-in-python</t>
         </is>
       </c>
     </row>
@@ -1667,7 +1685,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Natural Language Processing with spaCy</t>
+          <t>Dimensionality Reduction in Python</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1677,7 +1695,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/natural-language-processing-with-spacy</t>
+          <t>https://app.datacamp.com/learn/courses/dimensionality-reduction-in-python</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1705,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Feature Engineering for NLP in Python</t>
+          <t>Preprocessing for Machine Learning in Python</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1697,7 +1715,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-nlp-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/preprocessing-for-machine-learning-in-python</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1725,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Introduction to Deep Learning with PyTorch</t>
+          <t>Machine Learning for Time Series Data in Python</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1717,7 +1735,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-deep-learning-with-pytorch</t>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-for-time-series-data-in-python</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1745,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Intermediate Deep Learning with PyTorch</t>
+          <t>Feature Engineering for Machine Learning in Python</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1737,7 +1755,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-deep-learning-with-pytorch</t>
+          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-machine-learning-in-python</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1765,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Image Processing in Python</t>
+          <t>Model Validation in Python</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1757,7 +1775,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/image-processing-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/model-validation-in-python</t>
         </is>
       </c>
     </row>
@@ -1767,7 +1785,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Introduction to PySpark</t>
+          <t>Hyperparameter Tuning in Python</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1777,7 +1795,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-pyspark</t>
+          <t>https://app.datacamp.com/learn/courses/hyperparameter-tuning-in-python</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1805,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Machine Learning with PySpark</t>
+          <t>Introduction to Natural Language Processing in Python</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1797,7 +1815,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/machine-learning-with-pyspark</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-natural-language-processing-in-python</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1825,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Winning a Kaggle Competition in Python</t>
+          <t>Natural Language Processing with spaCy</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1817,7 +1835,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/winning-a-kaggle-competition-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/natural-language-processing-with-spacy</t>
         </is>
       </c>
     </row>
@@ -1827,17 +1845,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Introduction to SQL</t>
+          <t>Feature Engineering for NLP in Python</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-sql</t>
+          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-nlp-in-python</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1865,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Intermediate SQL</t>
+          <t>Introduction to Deep Learning with PyTorch</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1857,7 +1875,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-sql</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-deep-learning-with-pytorch</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1885,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Joining Data in SQL</t>
+          <t>Intermediate Deep Learning with PyTorch</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1877,7 +1895,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/joining-data-in-sql</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-deep-learning-with-pytorch</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1905,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Data Manipulation in SQL</t>
+          <t>Image Processing in Python</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1897,7 +1915,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-manipulation-in-sql</t>
+          <t>https://app.datacamp.com/learn/courses/image-processing-in-python</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1925,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>PostgreSQL Summary Stats and Window Functions</t>
+          <t>Introduction to PySpark</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1917,7 +1935,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/postgresql-summary-stats-and-window-functions</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-pyspark</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1945,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Functions for Manipulating Data in PostgreSQL</t>
+          <t>Machine Learning with PySpark</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1937,7 +1955,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/functions-for-manipulating-data-in-postgresql</t>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-with-pyspark</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1965,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Database Design</t>
+          <t>Winning a Kaggle Competition in Python</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1957,7 +1975,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/database-design</t>
+          <t>https://app.datacamp.com/learn/courses/winning-a-kaggle-competition-in-python</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1985,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Time Series Analysis in Python</t>
+          <t>Data Manipulation in SQL</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1977,7 +1995,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/time-series-analysis-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/data-manipulation-in-sql</t>
         </is>
       </c>
     </row>
@@ -1987,7 +2005,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Visualizing Time Series Data in Python</t>
+          <t>PostgreSQL Summary Stats and Window Functions</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1997,7 +2015,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/visualizing-time-series-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/postgresql-summary-stats-and-window-functions</t>
         </is>
       </c>
     </row>
@@ -2007,15 +2025,95 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>Functions for Manipulating Data in PostgreSQL</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/functions-for-manipulating-data-in-postgresql</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Database Design</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/database-design</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Time Series Analysis in Python</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/time-series-analysis-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Visualizing Time Series Data in Python</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/visualizing-time-series-data-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>ARIMA Models in Python</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>4 hr</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
         <is>
           <t>https://app.datacamp.com/learn/courses/arima-models-in-python</t>
         </is>
@@ -2032,7 +2130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2391,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
@@ -2403,7 +2501,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
@@ -2415,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
@@ -2427,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
@@ -2439,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
@@ -2448,10 +2546,10 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
@@ -2460,10 +2558,10 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
@@ -2472,10 +2570,10 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
@@ -2484,10 +2582,10 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" t="n">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
@@ -2496,10 +2594,10 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
@@ -2508,10 +2606,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
@@ -2520,10 +2618,10 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B40" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
@@ -2532,10 +2630,10 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
@@ -2544,10 +2642,10 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B42" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
@@ -2556,10 +2654,10 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
@@ -2568,10 +2666,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B44" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
@@ -2580,10 +2678,10 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B45" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
@@ -2592,10 +2690,10 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B46" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="n">
@@ -2604,10 +2702,10 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B47" t="n">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
@@ -2616,10 +2714,10 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B48" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
@@ -2628,10 +2726,10 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B49" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
@@ -2640,10 +2738,10 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B50" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="n">
@@ -2652,10 +2750,10 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B51" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
@@ -2664,10 +2762,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B52" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
@@ -2676,10 +2774,10 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B53" t="n">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="n">
@@ -2688,10 +2786,10 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B54" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="n">
@@ -2700,10 +2798,10 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B55" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
@@ -2712,10 +2810,10 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B56" t="n">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="n">
@@ -2724,10 +2822,10 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B57" t="n">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="n">
@@ -2736,10 +2834,10 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B58" t="n">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="n">
@@ -2748,10 +2846,10 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B59" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
@@ -2760,10 +2858,10 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B60" t="n">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
@@ -2772,10 +2870,10 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B61" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
@@ -2784,10 +2882,10 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B62" t="n">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="n">
@@ -2796,10 +2894,10 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="n">
@@ -2808,10 +2906,10 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B64" t="n">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="n">
@@ -2820,10 +2918,10 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B65" t="n">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="n">
@@ -2832,10 +2930,10 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66" t="n">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
@@ -2844,10 +2942,10 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B67" t="n">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
@@ -2856,10 +2954,10 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B68" t="n">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="n">
@@ -2871,7 +2969,7 @@
         <v>6</v>
       </c>
       <c r="B69" t="n">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
@@ -2883,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="B70" t="n">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="n">
@@ -2892,10 +2990,10 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B71" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="n">
@@ -2904,10 +3002,10 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B72" t="n">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="n">
@@ -2916,10 +3014,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B73" t="n">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="n">
@@ -2928,10 +3026,10 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B74" t="n">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="n">
@@ -2940,13 +3038,325 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B75" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>6</v>
+      </c>
+      <c r="B76" t="n">
+        <v>52</v>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>6</v>
+      </c>
+      <c r="B77" t="n">
+        <v>53</v>
+      </c>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>6</v>
+      </c>
+      <c r="B78" t="n">
+        <v>54</v>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>6</v>
+      </c>
+      <c r="B79" t="n">
+        <v>55</v>
+      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>6</v>
+      </c>
+      <c r="B80" t="n">
+        <v>56</v>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>6</v>
+      </c>
+      <c r="B81" t="n">
+        <v>57</v>
+      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>6</v>
+      </c>
+      <c r="B82" t="n">
+        <v>58</v>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>6</v>
+      </c>
+      <c r="B83" t="n">
+        <v>59</v>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>6</v>
+      </c>
+      <c r="B84" t="n">
+        <v>60</v>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>6</v>
+      </c>
+      <c r="B85" t="n">
+        <v>61</v>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>6</v>
+      </c>
+      <c r="B86" t="n">
+        <v>62</v>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>6</v>
+      </c>
+      <c r="B87" t="n">
+        <v>63</v>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>6</v>
+      </c>
+      <c r="B88" t="n">
+        <v>64</v>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>6</v>
+      </c>
+      <c r="B89" t="n">
+        <v>65</v>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>7</v>
+      </c>
+      <c r="B90" t="n">
+        <v>33</v>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>7</v>
+      </c>
+      <c r="B91" t="n">
+        <v>34</v>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>7</v>
+      </c>
+      <c r="B92" t="n">
+        <v>35</v>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>7</v>
+      </c>
+      <c r="B93" t="n">
+        <v>66</v>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>7</v>
+      </c>
+      <c r="B94" t="n">
+        <v>67</v>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>7</v>
+      </c>
+      <c r="B95" t="n">
+        <v>68</v>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>7</v>
+      </c>
+      <c r="B96" t="n">
+        <v>69</v>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>8</v>
+      </c>
+      <c r="B97" t="n">
+        <v>44</v>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>8</v>
+      </c>
+      <c r="B98" t="n">
+        <v>70</v>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>8</v>
+      </c>
+      <c r="B99" t="n">
+        <v>71</v>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>8</v>
+      </c>
+      <c r="B100" t="n">
+        <v>72</v>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>8</v>
+      </c>
+      <c r="B101" t="n">
+        <v>53</v>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusão da Capacitação avançada 2025
</commit_message>
<xml_diff>
--- a/data/arquivo.xlsx
+++ b/data/arquivo.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,16 +502,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Capacitação Básica 2025</t>
+          <t>Excel Fundamentals</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/capacitação-básica-2025</t>
+          <t>https://app.datacamp.com/learn/career-tracks/excel-fundamentals</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -520,12 +520,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Excel Fundamentals</t>
+          <t>Finance Fundamentals in Python</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/excel-fundamentals</t>
+          <t>https://app.datacamp.com/learn/career-tracks/finance-fundamentals-in-python</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -538,12 +538,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Finance Fundamentals in Python</t>
+          <t>Git Fundamentals</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/finance-fundamentals-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/git-fundamentals</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -556,12 +556,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Git Fundamentals</t>
+          <t>Machine Learning Scientist in Python</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/git-fundamentals</t>
+          <t>https://app.datacamp.com/learn/career-tracks/machine-learning-scientist-in-python</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -574,12 +574,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Machine Learning Scientist in Python</t>
+          <t>SQL Fundamentals</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/machine-learning-scientist-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/sql-fundamentals</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -592,12 +592,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SQL Fundamentals</t>
+          <t>Time Series in Python</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/sql-fundamentals</t>
+          <t>https://app.datacamp.com/learn/career-tracks/time-series-in-python</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -610,16 +610,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Time Series in Python</t>
+          <t>Capacitação Avançada 2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/time-series-in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/capacitação-avançada-2025</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Capacitação Básica 2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/capacitação-básica-2025</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1209,17 +1227,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Introduction to Git</t>
+          <t>Introduction to Excel</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-git</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-excel</t>
         </is>
       </c>
     </row>
@@ -1229,17 +1247,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Introduction to Data Visualization with Plotly in Python</t>
+          <t>Data Preparation in Excel</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-data-visualization-with-plotly-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/data-preparation-in-excel</t>
         </is>
       </c>
     </row>
@@ -1249,17 +1267,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Intermediate Git</t>
+          <t>Data Visualization in Excel</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-git</t>
+          <t>https://app.datacamp.com/learn/courses/data-visualization-in-excel</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1287,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Introduction to Object-Oriented Programming in Python</t>
+          <t>Data Analysis in Excel</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1279,7 +1297,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-object-oriented-programming-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/data-analysis-in-excel</t>
         </is>
       </c>
     </row>
@@ -1289,17 +1307,13 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Intermediate Object-Oriented Programming in Python</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>4 hr</t>
-        </is>
-      </c>
+          <t>Case Study: Analyzing Customer Churn in Excel</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-object-oriented-programming-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/case-study:-analyzing-customer-churn-in-excel</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1323,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Web Scraping in Python</t>
+          <t>Introduction to Python for Finance</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1319,7 +1333,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/web-scraping-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-python-for-finance</t>
         </is>
       </c>
     </row>
@@ -1329,17 +1343,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Introduction to SQL</t>
+          <t>Intermediate Python for Finance</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-sql</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-python-for-finance</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1363,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Intermediate SQL</t>
+          <t>Introduction to Financial Concepts in Python</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1359,7 +1373,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-sql</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-financial-concepts-in-python</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1383,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Joining Data in SQL</t>
+          <t>Manipulating Time Series Data in Python</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1379,7 +1393,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/joining-data-in-sql</t>
+          <t>https://app.datacamp.com/learn/courses/manipulating-time-series-data-in-python</t>
         </is>
       </c>
     </row>
@@ -1389,17 +1403,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Introduction to Excel</t>
+          <t>Importing and Managing Financial Data in Python</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>5 hr</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-excel</t>
+          <t>https://app.datacamp.com/learn/courses/importing-and-managing-financial-data-in-python</t>
         </is>
       </c>
     </row>
@@ -1409,17 +1423,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Data Preparation in Excel</t>
+          <t>Introduction to Portfolio Analysis in Python</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>3 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-preparation-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-portfolio-analysis-in-python</t>
         </is>
       </c>
     </row>
@@ -1429,17 +1443,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Data Visualization in Excel</t>
+          <t>Introduction to Git</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3 hr</t>
+          <t>2 hr</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-visualization-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-git</t>
         </is>
       </c>
     </row>
@@ -1449,17 +1463,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Data Analysis in Excel</t>
+          <t>Intermediate Git</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3 hr</t>
+          <t>2 hr</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-analysis-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-git</t>
         </is>
       </c>
     </row>
@@ -1469,13 +1483,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Case Study: Analyzing Customer Churn in Excel</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr"/>
+          <t>Advanced Git</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3 hr</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/case-study:-analyzing-customer-churn-in-excel</t>
+          <t>https://app.datacamp.com/learn/courses/advanced-git</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1503,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Introduction to Python for Finance</t>
+          <t>Linear Classifiers in Python</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1495,7 +1513,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-python-for-finance</t>
+          <t>https://app.datacamp.com/learn/courses/linear-classifiers-in-python</t>
         </is>
       </c>
     </row>
@@ -1505,7 +1523,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Intermediate Python for Finance</t>
+          <t>Extreme Gradient Boosting with XGBoost</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1515,7 +1533,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-python-for-finance</t>
+          <t>https://app.datacamp.com/learn/courses/extreme-gradient-boosting-with-xgboost</t>
         </is>
       </c>
     </row>
@@ -1525,7 +1543,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Introduction to Financial Concepts in Python</t>
+          <t>Cluster Analysis in Python</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1535,7 +1553,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-financial-concepts-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/cluster-analysis-in-python</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1563,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Manipulating Time Series Data in Python</t>
+          <t>Dimensionality Reduction in Python</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1555,7 +1573,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/manipulating-time-series-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/dimensionality-reduction-in-python</t>
         </is>
       </c>
     </row>
@@ -1565,17 +1583,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Importing and Managing Financial Data in Python</t>
+          <t>Preprocessing for Machine Learning in Python</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>5 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/importing-and-managing-financial-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/preprocessing-for-machine-learning-in-python</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1603,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Introduction to Portfolio Analysis in Python</t>
+          <t>Machine Learning for Time Series Data in Python</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1595,7 +1613,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-portfolio-analysis-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-for-time-series-data-in-python</t>
         </is>
       </c>
     </row>
@@ -1605,17 +1623,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Advanced Git</t>
+          <t>Feature Engineering for Machine Learning in Python</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>3 hr</t>
+          <t>4 hr</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/advanced-git</t>
+          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-machine-learning-in-python</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1643,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Linear Classifiers in Python</t>
+          <t>Model Validation in Python</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1635,7 +1653,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/linear-classifiers-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/model-validation-in-python</t>
         </is>
       </c>
     </row>
@@ -1645,7 +1663,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Extreme Gradient Boosting with XGBoost</t>
+          <t>Hyperparameter Tuning in Python</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1655,7 +1673,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/extreme-gradient-boosting-with-xgboost</t>
+          <t>https://app.datacamp.com/learn/courses/hyperparameter-tuning-in-python</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1683,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Cluster Analysis in Python</t>
+          <t>Introduction to Natural Language Processing in Python</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1675,7 +1693,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/cluster-analysis-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-natural-language-processing-in-python</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1703,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Dimensionality Reduction in Python</t>
+          <t>Natural Language Processing with spaCy</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1695,7 +1713,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/dimensionality-reduction-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/natural-language-processing-with-spacy</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1723,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Preprocessing for Machine Learning in Python</t>
+          <t>Feature Engineering for NLP in Python</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1715,7 +1733,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/preprocessing-for-machine-learning-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-nlp-in-python</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1743,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Machine Learning for Time Series Data in Python</t>
+          <t>Introduction to Deep Learning with PyTorch</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1735,7 +1753,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/machine-learning-for-time-series-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-deep-learning-with-pytorch</t>
         </is>
       </c>
     </row>
@@ -1745,7 +1763,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Feature Engineering for Machine Learning in Python</t>
+          <t>Intermediate Deep Learning with PyTorch</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1755,7 +1773,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-machine-learning-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-deep-learning-with-pytorch</t>
         </is>
       </c>
     </row>
@@ -1765,7 +1783,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Model Validation in Python</t>
+          <t>Image Processing in Python</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1775,7 +1793,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/model-validation-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/image-processing-in-python</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1803,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Hyperparameter Tuning in Python</t>
+          <t>Introduction to PySpark</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1795,7 +1813,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/hyperparameter-tuning-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-pyspark</t>
         </is>
       </c>
     </row>
@@ -1805,7 +1823,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Introduction to Natural Language Processing in Python</t>
+          <t>Machine Learning with PySpark</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1815,7 +1833,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-natural-language-processing-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/machine-learning-with-pyspark</t>
         </is>
       </c>
     </row>
@@ -1825,7 +1843,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Natural Language Processing with spaCy</t>
+          <t>Winning a Kaggle Competition in Python</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1835,7 +1853,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/natural-language-processing-with-spacy</t>
+          <t>https://app.datacamp.com/learn/courses/winning-a-kaggle-competition-in-python</t>
         </is>
       </c>
     </row>
@@ -1845,17 +1863,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Feature Engineering for NLP in Python</t>
+          <t>Introduction to SQL</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>2 hr</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/feature-engineering-for-nlp-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-sql</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1883,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Introduction to Deep Learning with PyTorch</t>
+          <t>Intermediate SQL</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1875,7 +1893,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-deep-learning-with-pytorch</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-sql</t>
         </is>
       </c>
     </row>
@@ -1885,7 +1903,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Intermediate Deep Learning with PyTorch</t>
+          <t>Joining Data in SQL</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1895,7 +1913,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/intermediate-deep-learning-with-pytorch</t>
+          <t>https://app.datacamp.com/learn/courses/joining-data-in-sql</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1923,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Image Processing in Python</t>
+          <t>Data Manipulation in SQL</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1915,7 +1933,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/image-processing-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/data-manipulation-in-sql</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1943,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Introduction to PySpark</t>
+          <t>PostgreSQL Summary Stats and Window Functions</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1935,7 +1953,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/introduction-to-pyspark</t>
+          <t>https://app.datacamp.com/learn/courses/postgresql-summary-stats-and-window-functions</t>
         </is>
       </c>
     </row>
@@ -1945,7 +1963,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Machine Learning with PySpark</t>
+          <t>Functions for Manipulating Data in PostgreSQL</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1955,7 +1973,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/machine-learning-with-pyspark</t>
+          <t>https://app.datacamp.com/learn/courses/functions-for-manipulating-data-in-postgresql</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1983,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Winning a Kaggle Competition in Python</t>
+          <t>Database Design</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1975,7 +1993,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/winning-a-kaggle-competition-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/database-design</t>
         </is>
       </c>
     </row>
@@ -1985,7 +2003,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Data Manipulation in SQL</t>
+          <t>Time Series Analysis in Python</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1995,7 +2013,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/data-manipulation-in-sql</t>
+          <t>https://app.datacamp.com/learn/courses/time-series-analysis-in-python</t>
         </is>
       </c>
     </row>
@@ -2005,7 +2023,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>PostgreSQL Summary Stats and Window Functions</t>
+          <t>Visualizing Time Series Data in Python</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2015,7 +2033,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/postgresql-summary-stats-and-window-functions</t>
+          <t>https://app.datacamp.com/learn/courses/visualizing-time-series-data-in-python</t>
         </is>
       </c>
     </row>
@@ -2025,7 +2043,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Functions for Manipulating Data in PostgreSQL</t>
+          <t>ARIMA Models in Python</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2035,7 +2053,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/functions-for-manipulating-data-in-postgresql</t>
+          <t>https://app.datacamp.com/learn/courses/arima-models-in-python</t>
         </is>
       </c>
     </row>
@@ -2045,7 +2063,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Database Design</t>
+          <t>Web Scraping in Python</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2055,7 +2073,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/database-design</t>
+          <t>https://app.datacamp.com/learn/courses/web-scraping-in-python</t>
         </is>
       </c>
     </row>
@@ -2065,17 +2083,17 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Time Series Analysis in Python</t>
+          <t>Introduction to Object-Oriented Programming in Python</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>4 hr</t>
+          <t>3 hr</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/time-series-analysis-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-object-oriented-programming-in-python</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2103,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Visualizing Time Series Data in Python</t>
+          <t>Intermediate Object-Oriented Programming in Python</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2095,7 +2113,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/visualizing-time-series-data-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/intermediate-object-oriented-programming-in-python</t>
         </is>
       </c>
     </row>
@@ -2105,7 +2123,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ARIMA Models in Python</t>
+          <t>Introduction to Optimization in Python</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2115,7 +2133,47 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/courses/arima-models-in-python</t>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-optimization-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Introduction to Deep Learning in Python</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-deep-learning-in-python</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Introduction to Data Visualization with Plotly in Python</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>4 hr</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/courses/introduction-to-data-visualization-with-plotly-in-python</t>
         </is>
       </c>
     </row>
@@ -2130,7 +2188,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2486,10 +2544,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
@@ -2498,10 +2556,10 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
@@ -2510,10 +2568,10 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B31" t="n">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
@@ -2522,10 +2580,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B32" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
@@ -2534,10 +2592,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
@@ -2546,10 +2604,10 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B34" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
@@ -2558,10 +2616,10 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B35" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
@@ -2570,10 +2628,10 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B36" t="n">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
@@ -2582,10 +2640,10 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B37" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
@@ -2594,10 +2652,10 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B38" t="n">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
@@ -2606,10 +2664,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B39" t="n">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
@@ -2618,10 +2676,10 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B40" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
@@ -2630,10 +2688,10 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B41" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
@@ -2642,10 +2700,10 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B42" t="n">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
@@ -2654,10 +2712,10 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B43" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
@@ -2666,10 +2724,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B44" t="n">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
@@ -2678,10 +2736,10 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B45" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
@@ -2690,10 +2748,10 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B46" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="n">
@@ -2702,10 +2760,10 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B47" t="n">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
@@ -2714,10 +2772,10 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B48" t="n">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
@@ -2726,10 +2784,10 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B49" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
@@ -2738,10 +2796,10 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B50" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="n">
@@ -2750,10 +2808,10 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B51" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
@@ -2762,10 +2820,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B52" t="n">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
@@ -2774,7 +2832,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B53" t="n">
         <v>38</v>
@@ -2786,10 +2844,10 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B54" t="n">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="n">
@@ -2798,10 +2856,10 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B55" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
@@ -2810,10 +2868,10 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B56" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="n">
@@ -2822,10 +2880,10 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B57" t="n">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="n">
@@ -2834,10 +2892,10 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B58" t="n">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="n">
@@ -2846,10 +2904,10 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B59" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
@@ -2858,10 +2916,10 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B60" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
@@ -2870,10 +2928,10 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B61" t="n">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
@@ -2882,10 +2940,10 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B62" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="n">
@@ -2894,10 +2952,10 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B63" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="n">
@@ -2906,10 +2964,10 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B64" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="n">
@@ -2918,10 +2976,10 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B65" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="n">
@@ -2930,10 +2988,10 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B66" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
@@ -2942,10 +3000,10 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B67" t="n">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
@@ -2954,10 +3012,10 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B68" t="n">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="n">
@@ -2966,10 +3024,10 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B69" t="n">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
@@ -2978,10 +3036,10 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B70" t="n">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="n">
@@ -2990,10 +3048,10 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B71" t="n">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="n">
@@ -3002,10 +3060,10 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B72" t="n">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="n">
@@ -3014,10 +3072,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B73" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="n">
@@ -3026,10 +3084,10 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B74" t="n">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="n">
@@ -3038,10 +3096,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B75" t="n">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="n">
@@ -3050,10 +3108,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B76" t="n">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
@@ -3062,10 +3120,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B77" t="n">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="n">
@@ -3074,10 +3132,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B78" t="n">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="n">
@@ -3086,10 +3144,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B79" t="n">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
@@ -3098,10 +3156,10 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B80" t="n">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="n">
@@ -3110,10 +3168,10 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B81" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="n">
@@ -3122,10 +3180,10 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B82" t="n">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="n">
@@ -3134,10 +3192,10 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B83" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="n">
@@ -3146,10 +3204,10 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B84" t="n">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="n">
@@ -3158,10 +3216,10 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B85" t="n">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="n">
@@ -3170,10 +3228,10 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B86" t="n">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
@@ -3182,10 +3240,10 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B87" t="n">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="n">
@@ -3194,10 +3252,10 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B88" t="n">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="n">
@@ -3206,10 +3264,10 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B89" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="n">
@@ -3218,10 +3276,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B90" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="n">
@@ -3230,10 +3288,10 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B91" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="n">
@@ -3242,10 +3300,10 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B92" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="n">
@@ -3254,10 +3312,10 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B93" t="n">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="n">
@@ -3266,10 +3324,10 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B94" t="n">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="n">
@@ -3278,10 +3336,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B95" t="n">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="n">
@@ -3290,10 +3348,10 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B96" t="n">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="n">
@@ -3302,7 +3360,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B97" t="n">
         <v>44</v>
@@ -3314,10 +3372,10 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B98" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="n">
@@ -3326,10 +3384,10 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B99" t="n">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="n">
@@ -3338,10 +3396,10 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B100" t="n">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="n">
@@ -3350,13 +3408,277 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B101" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>5</v>
+      </c>
+      <c r="B102" t="n">
+        <v>49</v>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>5</v>
+      </c>
+      <c r="B103" t="n">
+        <v>50</v>
+      </c>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>5</v>
+      </c>
+      <c r="B104" t="n">
+        <v>51</v>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>5</v>
+      </c>
+      <c r="B105" t="n">
+        <v>52</v>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>5</v>
+      </c>
+      <c r="B106" t="n">
+        <v>53</v>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>5</v>
+      </c>
+      <c r="B107" t="n">
+        <v>54</v>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>5</v>
+      </c>
+      <c r="B108" t="n">
+        <v>55</v>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>5</v>
+      </c>
+      <c r="B109" t="n">
+        <v>56</v>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>5</v>
+      </c>
+      <c r="B110" t="n">
+        <v>57</v>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>5</v>
+      </c>
+      <c r="B111" t="n">
+        <v>58</v>
+      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>6</v>
+      </c>
+      <c r="B112" t="n">
+        <v>59</v>
+      </c>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>6</v>
+      </c>
+      <c r="B113" t="n">
+        <v>60</v>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>6</v>
+      </c>
+      <c r="B114" t="n">
+        <v>61</v>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>6</v>
+      </c>
+      <c r="B115" t="n">
+        <v>62</v>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>6</v>
+      </c>
+      <c r="B116" t="n">
+        <v>63</v>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>6</v>
+      </c>
+      <c r="B117" t="n">
+        <v>64</v>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>6</v>
+      </c>
+      <c r="B118" t="n">
+        <v>65</v>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>7</v>
+      </c>
+      <c r="B119" t="n">
+        <v>35</v>
+      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>7</v>
+      </c>
+      <c r="B120" t="n">
+        <v>66</v>
+      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>7</v>
+      </c>
+      <c r="B121" t="n">
+        <v>67</v>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>7</v>
+      </c>
+      <c r="B122" t="n">
+        <v>68</v>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>7</v>
+      </c>
+      <c r="B123" t="n">
+        <v>46</v>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>